<commit_message>
SwitchNetwork Finished. Gerber/BOM/P&P generated
</commit_message>
<xml_diff>
--- a/src/schematics/Ard_Shield/Gerber/ScouseTom_New_Pick_and_Place.xlsx
+++ b/src/schematics/Ard_Shield/Gerber/ScouseTom_New_Pick_and_Place.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="100">
   <si>
     <t>C1</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>Top</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1179,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,10 +1210,10 @@
         <v>81</v>
       </c>
       <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
       </c>
       <c r="G1" t="s">
         <v>84</v>

</xml_diff>